<commit_message>
Updated graphs, repot and FuzzyCar
</commit_message>
<xml_diff>
--- a/Fuzzy Graphs.xlsx
+++ b/Fuzzy Graphs.xlsx
@@ -175,8 +175,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>MATLAB - Velocity = 0</a:t>
+              <a:t>MATLAB - Velocity</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> = 0</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -245,29 +250,41 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$7</c:f>
+              <c:f>Sheet1!$A$1:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-0.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -275,30 +292,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$7</c:f>
+              <c:f>Sheet1!$B$1:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.48399999999999999</c:v>
+                  <c:v>-0.42299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.47</c:v>
+                  <c:v>-0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.25700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>1.53E-17</c:v>
+                  <c:v>-0.41699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                  <c:v>-0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>8.0099999999999997E-18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48399999999999999</c:v>
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42299999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,7 +335,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3650-4E76-A9CF-1624488EACAD}"/>
+              <c16:uniqueId val="{00000000-E22B-4A1C-8E8B-6BF0CCD22093}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -318,11 +347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="479459256"/>
-        <c:axId val="479461224"/>
+        <c:axId val="618558688"/>
+        <c:axId val="618560328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="479459256"/>
+        <c:axId val="618558688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,12 +464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479461224"/>
+        <c:crossAx val="618560328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="479461224"/>
+        <c:axId val="618560328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479459256"/>
+        <c:crossAx val="618558688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -637,13 +666,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>MATLAB - Distance</a:t>
+              <a:t>MATLAB - Distance = 0</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> = 0</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -712,29 +736,41 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$23</c:f>
+              <c:f>Sheet1!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-0.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -742,30 +778,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$23</c:f>
+              <c:f>Sheet1!$B$17:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.48399999999999999</c:v>
+                  <c:v>-0.42299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.47</c:v>
+                  <c:v>-0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.25700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>1.53E-17</c:v>
+                  <c:v>-0.41699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                  <c:v>-0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>8.0099999999999997E-18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48399999999999999</c:v>
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42299999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -773,7 +821,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6B37-4F7C-AD91-305AA3EF25E7}"/>
+              <c16:uniqueId val="{00000000-8E92-4D9F-931B-9CA783B437CF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -785,11 +833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="546661728"/>
-        <c:axId val="546657464"/>
+        <c:axId val="622098512"/>
+        <c:axId val="622098840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="546661728"/>
+        <c:axId val="622098512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,12 +950,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="546657464"/>
+        <c:crossAx val="622098840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="546657464"/>
+        <c:axId val="622098840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="546661728"/>
+        <c:crossAx val="622098512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1104,13 +1152,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Application</a:t>
+              <a:t>Application - Velocity = 0</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> - Velocity = 0</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1179,29 +1222,41 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$32:$A$38</c:f>
+              <c:f>Sheet1!$A$32:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-0.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1209,30 +1264,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$B$38</c:f>
+              <c:f>Sheet1!$B$32:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.49399999999999999</c:v>
+                  <c:v>-0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.48899999999999999</c:v>
+                  <c:v>-0.42099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>-1.1869999999999999E-17</c:v>
+                  <c:v>-0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.48899999999999999</c:v>
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>-3.231E-18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49399999999999999</c:v>
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,7 +1307,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E491-44D1-9097-5010DF71403B}"/>
+              <c16:uniqueId val="{00000000-FA4D-43B0-9EA6-6EF9EBF6298A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1252,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="553578808"/>
-        <c:axId val="553579136"/>
+        <c:axId val="616196224"/>
+        <c:axId val="616200160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="553578808"/>
+        <c:axId val="616196224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,12 +1436,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553579136"/>
+        <c:crossAx val="616200160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="553579136"/>
+        <c:axId val="616200160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1554,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553578808"/>
+        <c:crossAx val="616196224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1641,29 +1708,41 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$47:$A$53</c:f>
+              <c:f>Sheet1!$A$47:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-0.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1671,30 +1750,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$47:$B$53</c:f>
+              <c:f>Sheet1!$B$47:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.47299999999999998</c:v>
+                  <c:v>-0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.45</c:v>
+                  <c:v>-0.42099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.186</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>-1.1869999999999999E-17</c:v>
+                  <c:v>-0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>-3.231E-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.186</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.47299999999999998</c:v>
+                <c:pt idx="7">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1702,7 +1793,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0C43-4518-8D20-6DB16F8A1169}"/>
+              <c16:uniqueId val="{00000000-1831-49D5-8FD1-F5A8230F8767}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1714,11 +1805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="553994248"/>
-        <c:axId val="553993592"/>
+        <c:axId val="672224272"/>
+        <c:axId val="672231488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="553994248"/>
+        <c:axId val="672224272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,12 +1922,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553993592"/>
+        <c:crossAx val="672231488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="553993592"/>
+        <c:axId val="672231488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +2040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553994248"/>
+        <c:crossAx val="672224272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4227,19 +4318,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4257,19 +4348,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4287,19 +4378,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4317,19 +4408,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>557212</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4610,10 +4701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4623,55 +4714,87 @@
         <v>-1</v>
       </c>
       <c r="B1" s="2">
-        <v>-0.48399999999999999</v>
+        <v>-0.42299999999999999</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="B2" s="4">
-        <v>-0.47</v>
+        <v>-0.42199999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.25700000000000001</v>
+        <v>-0.41699999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1.53E-17</v>
+        <v>-0.25</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-0.38500000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="B5" s="4">
-        <v>0.25700000000000001</v>
+        <v>-0.14299999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8.0099999999999997E-18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="4">
-        <v>0.48399999999999999</v>
+      <c r="B11" s="4">
+        <v>0.42299999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4680,55 +4803,87 @@
         <v>-1</v>
       </c>
       <c r="B17" s="2">
-        <v>-0.48399999999999999</v>
+        <v>-0.42299999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="B18" s="4">
-        <v>-0.47</v>
+        <v>-0.42199999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="B19" s="4">
-        <v>-0.25700000000000001</v>
+        <v>-0.41699999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>0</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1.53E-17</v>
+        <v>-0.25</v>
+      </c>
+      <c r="B20" s="4">
+        <v>-0.38500000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="B21" s="4">
-        <v>0.25700000000000001</v>
+        <v>-0.14299999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>8.0099999999999997E-18</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>1</v>
       </c>
-      <c r="B23" s="4">
-        <v>0.48399999999999999</v>
+      <c r="B27" s="4">
+        <v>0.42299999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4737,55 +4892,87 @@
         <v>-1</v>
       </c>
       <c r="B32" s="2">
-        <v>-0.49399999999999999</v>
+        <v>-0.42199999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="B33" s="4">
-        <v>-0.48899999999999999</v>
+        <v>-0.42099999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="B34" s="4">
-        <v>-0.32</v>
+        <v>-0.41499999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>0</v>
-      </c>
-      <c r="B35" s="5">
-        <v>-1.1869999999999999E-17</v>
+        <v>-0.25</v>
+      </c>
+      <c r="B35" s="4">
+        <v>-0.38</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="B36" s="4">
-        <v>0.32</v>
+        <v>-0.14000000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B37" s="4">
-        <v>0.48899999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="B37" s="5">
+        <v>-3.231E-18</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>1</v>
       </c>
-      <c r="B38" s="4">
-        <v>0.49399999999999999</v>
+      <c r="B42" s="4">
+        <v>0.42199999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4794,60 +4981,92 @@
         <v>-1</v>
       </c>
       <c r="B47" s="2">
-        <v>-0.47299999999999998</v>
+        <v>-0.42199999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="B48" s="4">
-        <v>-0.45</v>
+        <v>-0.42099999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="B49" s="4">
-        <v>-0.186</v>
+        <v>-0.41499999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>0</v>
-      </c>
-      <c r="B50" s="5">
-        <v>-1.1869999999999999E-17</v>
+        <v>-0.25</v>
+      </c>
+      <c r="B50" s="4">
+        <v>-0.38</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="B51" s="4">
-        <v>0.186</v>
+        <v>-0.14000000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B52" s="4">
-        <v>0.45</v>
+        <v>0</v>
+      </c>
+      <c r="B52" s="5">
+        <v>-3.231E-18</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B53" s="4">
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
         <v>1</v>
       </c>
-      <c r="B53" s="4">
-        <v>0.47299999999999998</v>
+      <c r="B57" s="4">
+        <v>0.42199999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>